<commit_message>
Format tables in Markdown
</commit_message>
<xml_diff>
--- a/notebooks/Reopening_Indicators_Comparison.xlsx
+++ b/notebooks/Reopening_Indicators_Comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\404031\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\404031\Documents\GitHub\public-health-prototype\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,6 +87,198 @@
     <t>Share of Positive Tests</t>
   </si>
   <si>
+    <t>Share of positive results are decreasing below 15% of those tested in the community</t>
+  </si>
+  <si>
+    <t>Hospital Bed Availability</t>
+  </si>
+  <si>
+    <t>PPE</t>
+  </si>
+  <si>
+    <t>Testing Capacity</t>
+  </si>
+  <si>
+    <t>Contact Tracing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fewer than 1,800 coronavirus patients in hospital beds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fewer than 600 coronavirus patients in ICU beds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fewer than 450 coronavirus patients on ventilators</t>
+    </r>
+  </si>
+  <si>
+    <t>Test 135,000 per month, equivalent to 4,500 people per day (need to convert to per 1,000 rate per month)</t>
+  </si>
+  <si>
+    <t>Stable or declining rates of ICU deaths</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stable or declining rates of hospitalizations </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Stable or declining rates of ICU admissions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+  </si>
+  <si>
+    <t>White House Opening Up America Again - gating criteria</t>
+  </si>
+  <si>
+    <t>https://www.whitehouse.gov/wp-content/uploads/2020/04/Guidelines-for-Opening-Up-America-Again.pdf</t>
+  </si>
+  <si>
+    <t>NY State Indicators</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2020/05/04/nyregion/coronavirus-reopen-cuomo-ny.html</t>
+  </si>
+  <si>
+    <t>https://www.governor.ny.gov/news/amid-ongoing-covid-19-pandemic-governor-cuomo-outlines-additional-guidelines-when-regions-can</t>
+  </si>
+  <si>
+    <t>NYT State Reopening Analysis</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/interactive/2020/05/07/us/coronavirus-states-reopen-criteria.html</t>
+  </si>
+  <si>
+    <t>Chicago Indicators</t>
+  </si>
+  <si>
+    <t>https://www.chicagotribune.com/coronavirus/ct-coronavirus-chicago-reopening-lightfoot-20200508-ztpnouwexrcvfdfcr2yccbc53a-story.html</t>
+  </si>
+  <si>
+    <r>
+      <t>At least 14 days decline in total net hospitalizations on a 3-day rolling average </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 
+Less than 15 net new total hospitalizations on a 3-day rolling average</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>At least 14 days decline in total net deaths on a 3-day rolling average </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 
+Less than 5 new deaths on a 3-day rolling average</t>
+    </r>
+  </si>
+  <si>
+    <t>White House Gating Criteria</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">At least 14 days decline in new cases, on average </t>
     </r>
@@ -132,214 +324,15 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-A t least 14 days decline in rate of new cases (per capita?) </t>
-    </r>
-  </si>
-  <si>
-    <t>Share of positive results are decreasing below 15% of those tested in the community</t>
-  </si>
-  <si>
-    <t>Hospital Bed Availability</t>
-  </si>
-  <si>
-    <t>PPE</t>
-  </si>
-  <si>
-    <t>Testing Capacity</t>
-  </si>
-  <si>
-    <t>Contact Tracing</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fewer than 1,800 coronavirus patients in hospital beds </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Fewer than 600 coronavirus patients in ICU beds </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Fewer than 450 coronavirus patients on ventilators</t>
-    </r>
-  </si>
-  <si>
-    <t>Test 135,000 per month, equivalent to 4,500 people per day (need to convert to per 1,000 rate per month)</t>
-  </si>
-  <si>
-    <t>Stable or declining rates of ICU deaths</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Stable or declining rates of hospitalizations </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Stable or declining rates of ICU admissions </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-  </si>
-  <si>
-    <t>White House Opening Up America Again - gating criteria</t>
-  </si>
-  <si>
-    <t>https://www.whitehouse.gov/wp-content/uploads/2020/04/Guidelines-for-Opening-Up-America-Again.pdf</t>
-  </si>
-  <si>
-    <t>NY State Indicators</t>
-  </si>
-  <si>
-    <t>https://www.nytimes.com/2020/05/04/nyregion/coronavirus-reopen-cuomo-ny.html</t>
-  </si>
-  <si>
-    <t>https://www.governor.ny.gov/news/amid-ongoing-covid-19-pandemic-governor-cuomo-outlines-additional-guidelines-when-regions-can</t>
-  </si>
-  <si>
-    <t>NYT State Reopening Analysis</t>
-  </si>
-  <si>
-    <t>https://www.nytimes.com/interactive/2020/05/07/us/coronavirus-states-reopen-criteria.html</t>
-  </si>
-  <si>
-    <t>Chicago Indicators</t>
-  </si>
-  <si>
-    <t>https://www.chicagotribune.com/coronavirus/ct-coronavirus-chicago-reopening-lightfoot-20200508-ztpnouwexrcvfdfcr2yccbc53a-story.html</t>
-  </si>
-  <si>
-    <r>
-      <t>At least 14 days decline in total net hospitalizations on a 3-day rolling average </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> 
-Less than 15 net new total hospitalizations on a 3-day rolling average</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>At least 14 days decline in total net deaths on a 3-day rolling average </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> 
-Less than 5 new deaths on a 3-day rolling average</t>
-    </r>
-  </si>
-  <si>
-    <t>White House Gating Criteria</t>
+At least 14 days decline in rate of new cases (per capita?) </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,19 +446,49 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -474,36 +497,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,7 +805,7 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
@@ -825,132 +818,132 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="17" t="s">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -982,40 +975,40 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>